<commit_message>
Peltast Model/Skin, Phalanx, Allegiance, Intego Rescaling
</commit_message>
<xml_diff>
--- a/ShipStats.xlsx
+++ b/ShipStats.xlsx
@@ -1172,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,8 +1195,7 @@
     <col min="15" max="15" width="7" style="1" customWidth="1"/>
     <col min="16" max="16" width="5.85546875" style="1" customWidth="1"/>
     <col min="17" max="17" width="7" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="9.140625" style="1" customWidth="1"/>
     <col min="20" max="20" width="7.28515625" style="2" customWidth="1"/>
     <col min="21" max="22" width="9.140625" style="1"/>
     <col min="23" max="23" width="5.7109375" style="1" customWidth="1"/>
@@ -1344,7 +1343,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1635,7 +1634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -1718,7 +1717,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1822,7 +1821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -1905,7 +1904,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -2009,7 +2008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -2113,7 +2112,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
@@ -2217,7 +2216,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
@@ -2261,7 +2260,7 @@
         <v>8</v>
       </c>
       <c r="O11" s="1">
-        <v>1200</v>
+        <v>1700</v>
       </c>
       <c r="P11" s="1">
         <v>0</v>
@@ -2273,7 +2272,7 @@
         <v>0</v>
       </c>
       <c r="S11" s="1">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="T11" s="2">
         <v>12</v>
@@ -2321,7 +2320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -2425,7 +2424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -2550,7 +2549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
@@ -2633,7 +2632,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>30</v>
       </c>
@@ -2737,7 +2736,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>31</v>
       </c>
@@ -2820,7 +2819,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
@@ -2903,7 +2902,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
@@ -3007,7 +3006,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="19" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>34</v>
       </c>
@@ -3132,7 +3131,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>35</v>
       </c>
@@ -3236,7 +3235,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>36</v>
       </c>
@@ -3298,7 +3297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>37</v>
       </c>
@@ -3402,7 +3401,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>38</v>
       </c>
@@ -3506,7 +3505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -3610,7 +3609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -3714,7 +3713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>41</v>
       </c>
@@ -3797,7 +3796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>42</v>
       </c>
@@ -3880,7 +3879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>82</v>
       </c>
@@ -3942,7 +3941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
Shields & Income Scalar
</commit_message>
<xml_diff>
--- a/ShipStats.xlsx
+++ b/ShipStats.xlsx
@@ -1172,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2343,10 +2343,10 @@
         <v>110</v>
       </c>
       <c r="H12">
-        <v>5500</v>
+        <v>5900</v>
       </c>
       <c r="I12">
-        <v>5500</v>
+        <v>5900</v>
       </c>
       <c r="J12">
         <v>60</v>

</xml_diff>

<commit_message>
Adding Hapan Stats Part 1
</commit_message>
<xml_diff>
--- a/ShipStats.xlsx
+++ b/ShipStats.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Corey\Documents\My Games\Ironclad Games\Sins of a Solar Empire Rebellion\Mods-Rebellion v1.85 Dev\Ascendancy-Sins\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bane\Documents\My Games\Ironclad Games\Sins of a Solar Empire Rebellion\Mods-Rebellion v1.85 Dev\Ascendancy-Sins\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">information!$A$1:$AO$82</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="116">
   <si>
     <t>w1 Range</t>
   </si>
@@ -285,15 +288,6 @@
     <t>(IR) Katana</t>
   </si>
   <si>
-    <t>(HC) BattleDragon</t>
-  </si>
-  <si>
-    <t>(HC) NovaCruiser</t>
-  </si>
-  <si>
-    <t>(HC) StarHome</t>
-  </si>
-  <si>
     <t>"ION"</t>
   </si>
   <si>
@@ -328,12 +322,60 @@
   </si>
   <si>
     <t xml:space="preserve">(IR) VSDII </t>
+  </si>
+  <si>
+    <t>(HA) Ray</t>
+  </si>
+  <si>
+    <t>(HA) Flare</t>
+  </si>
+  <si>
+    <t>(HA) Beta</t>
+  </si>
+  <si>
+    <t>(HA) Express</t>
+  </si>
+  <si>
+    <t>(HA) Stella</t>
+  </si>
+  <si>
+    <t>(HA) Olanji</t>
+  </si>
+  <si>
+    <t>(HA) Charubah</t>
+  </si>
+  <si>
+    <t>(HA) Terephon</t>
+  </si>
+  <si>
+    <t>(HA) Corona</t>
+  </si>
+  <si>
+    <t>(HA) Neutron</t>
+  </si>
+  <si>
+    <t>(HA) Pulsar</t>
+  </si>
+  <si>
+    <t>(HA) Mist</t>
+  </si>
+  <si>
+    <t>(HA) Magnetar</t>
+  </si>
+  <si>
+    <t>(HA) BattleDragon</t>
+  </si>
+  <si>
+    <t>(HA) StarHome</t>
+  </si>
+  <si>
+    <t>(HA) NovaCruiser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -470,7 +512,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -662,6 +704,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -841,7 +889,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -849,6 +897,7 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1169,28 +1218,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO69"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AO82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <pane ySplit="19" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K84" sqref="K84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="2" max="2" width="1.7109375" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="7" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" customWidth="1"/>
-    <col min="12" max="12" width="7" customWidth="1"/>
-    <col min="13" max="13" width="3.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13" style="6" customWidth="1"/>
     <col min="15" max="15" width="7" style="1" customWidth="1"/>
     <col min="16" max="16" width="5.85546875" style="1" customWidth="1"/>
@@ -1343,7 +1394,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1426,7 +1477,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -1530,7 +1581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1634,7 +1685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -1717,7 +1768,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1904,7 +1955,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -2008,7 +2059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -2112,7 +2163,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
@@ -2216,7 +2267,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
@@ -2320,7 +2371,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -2424,7 +2475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -2549,7 +2600,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
@@ -2632,7 +2683,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>30</v>
       </c>
@@ -2736,7 +2787,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>31</v>
       </c>
@@ -2819,7 +2870,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
@@ -2902,7 +2953,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
@@ -3006,7 +3057,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>34</v>
       </c>
@@ -3796,7 +3847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>44</v>
       </c>
@@ -3879,7 +3930,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>49</v>
       </c>
@@ -3941,7 +3992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>52</v>
       </c>
@@ -4026,7 +4077,7 @@
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
@@ -4107,7 +4158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>63</v>
       </c>
@@ -4190,7 +4241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>65</v>
       </c>
@@ -4275,7 +4326,7 @@
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
@@ -4314,7 +4365,7 @@
         <v>1</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="O33">
         <v>0</v>
@@ -4347,7 +4398,7 @@
       <c r="AF33"/>
       <c r="AG33"/>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>59</v>
       </c>
@@ -4430,7 +4481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>68</v>
       </c>
@@ -4596,7 +4647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>46</v>
       </c>
@@ -4679,7 +4730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>47</v>
       </c>
@@ -4783,7 +4834,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>56</v>
       </c>
@@ -4887,7 +4938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>45</v>
       </c>
@@ -4991,7 +5042,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>57</v>
       </c>
@@ -5074,7 +5125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>58</v>
       </c>
@@ -5159,7 +5210,7 @@
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="B43" t="s">
         <v>5</v>
@@ -5261,7 +5312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>67</v>
       </c>
@@ -5367,7 +5418,7 @@
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B45" t="s">
         <v>5</v>
@@ -5406,7 +5457,7 @@
         <v>2</v>
       </c>
       <c r="N45" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="O45">
         <v>25</v>
@@ -5427,7 +5478,7 @@
         <v>4</v>
       </c>
       <c r="U45" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="V45">
         <v>18</v>
@@ -5456,7 +5507,7 @@
     </row>
     <row r="46" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B46" t="s">
         <v>5</v>
@@ -5495,7 +5546,7 @@
         <v>1</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="O46">
         <v>200</v>
@@ -5528,7 +5579,7 @@
       <c r="AF46"/>
       <c r="AG46"/>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>43</v>
       </c>
@@ -5632,7 +5683,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>51</v>
       </c>
@@ -5736,7 +5787,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>53</v>
       </c>
@@ -5904,7 +5955,7 @@
     </row>
     <row r="51" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="B51" t="s">
         <v>5</v>
@@ -6006,7 +6057,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>61</v>
       </c>
@@ -6047,7 +6098,7 @@
         <v>3</v>
       </c>
       <c r="N52" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="O52">
         <v>100</v>
@@ -6068,7 +6119,7 @@
         <v>4</v>
       </c>
       <c r="U52" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="V52">
         <v>150</v>
@@ -6089,7 +6140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>66</v>
       </c>
@@ -6195,7 +6246,7 @@
     </row>
     <row r="54" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B54" t="s">
         <v>5</v>
@@ -6234,7 +6285,7 @@
         <v>2</v>
       </c>
       <c r="N54" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="O54">
         <v>120</v>
@@ -6255,7 +6306,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="U54" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="V54">
         <v>210</v>
@@ -6282,7 +6333,7 @@
       <c r="AF54"/>
       <c r="AG54"/>
     </row>
-    <row r="55" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>48</v>
       </c>
@@ -6490,7 +6541,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="57" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>60</v>
       </c>
@@ -6573,7 +6624,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="58" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>69</v>
       </c>
@@ -6658,7 +6709,7 @@
     </row>
     <row r="59" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B59" t="s">
         <v>5</v>
@@ -6697,7 +6748,7 @@
         <v>2</v>
       </c>
       <c r="N59" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="O59">
         <v>100</v>
@@ -6718,7 +6769,7 @@
         <v>4</v>
       </c>
       <c r="U59" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="V59">
         <v>150</v>
@@ -6747,7 +6798,7 @@
     </row>
     <row r="60" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B60" t="s">
         <v>5</v>
@@ -6786,7 +6837,7 @@
         <v>1</v>
       </c>
       <c r="N60" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="O60">
         <v>175</v>
@@ -6819,7 +6870,7 @@
       <c r="AF60"/>
       <c r="AG60"/>
     </row>
-    <row r="61" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>54</v>
       </c>
@@ -6925,7 +6976,7 @@
     </row>
     <row r="62" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B62" t="s">
         <v>5</v>
@@ -6964,7 +7015,7 @@
         <v>3</v>
       </c>
       <c r="N62" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="O62">
         <v>90</v>
@@ -6985,7 +7036,7 @@
         <v>4</v>
       </c>
       <c r="U62" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="V62">
         <v>90</v>
@@ -7006,7 +7057,7 @@
         <v>4</v>
       </c>
       <c r="AB62" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="AC62">
         <v>650</v>
@@ -7027,7 +7078,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>55</v>
       </c>
@@ -7152,7 +7203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>62</v>
       </c>
@@ -7277,7 +7328,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>64</v>
       </c>
@@ -7362,7 +7413,7 @@
     </row>
     <row r="66" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B66" t="s">
         <v>5</v>
@@ -7401,7 +7452,7 @@
         <v>3</v>
       </c>
       <c r="N66" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="O66">
         <v>120</v>
@@ -7422,7 +7473,7 @@
         <v>4</v>
       </c>
       <c r="U66" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="V66">
         <v>120</v>
@@ -7443,7 +7494,7 @@
         <v>4</v>
       </c>
       <c r="AB66" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="AC66">
         <v>150</v>
@@ -7464,7 +7515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>82</v>
       </c>
@@ -7526,7 +7577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>83</v>
       </c>
@@ -7713,7 +7764,549 @@
         <v>4</v>
       </c>
     </row>
+    <row r="70" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B71" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71">
+        <v>200</v>
+      </c>
+      <c r="D71">
+        <v>30</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="G71">
+        <v>25</v>
+      </c>
+      <c r="H71">
+        <v>650</v>
+      </c>
+      <c r="I71">
+        <v>650</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>3.5</v>
+      </c>
+      <c r="L71">
+        <v>0.6</v>
+      </c>
+      <c r="M71" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B72" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72">
+        <v>220</v>
+      </c>
+      <c r="D72">
+        <v>40</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>2</v>
+      </c>
+      <c r="G72">
+        <v>25</v>
+      </c>
+      <c r="H72">
+        <v>1550</v>
+      </c>
+      <c r="I72">
+        <v>1550</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>2</v>
+      </c>
+      <c r="L72">
+        <v>0.6</v>
+      </c>
+      <c r="M72" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73">
+        <v>200</v>
+      </c>
+      <c r="D73">
+        <v>30</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="G73">
+        <v>25</v>
+      </c>
+      <c r="H73">
+        <v>1550</v>
+      </c>
+      <c r="I73">
+        <v>1550</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>2</v>
+      </c>
+      <c r="L73">
+        <v>0.6</v>
+      </c>
+      <c r="M73" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B74" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74">
+        <v>320</v>
+      </c>
+      <c r="D74">
+        <v>60</v>
+      </c>
+      <c r="E74">
+        <v>75</v>
+      </c>
+      <c r="F74">
+        <v>4</v>
+      </c>
+      <c r="G74">
+        <v>40</v>
+      </c>
+      <c r="H74">
+        <v>1750</v>
+      </c>
+      <c r="I74">
+        <v>1750</v>
+      </c>
+      <c r="J74">
+        <v>133</v>
+      </c>
+      <c r="K74">
+        <v>2</v>
+      </c>
+      <c r="L74">
+        <v>0.6</v>
+      </c>
+      <c r="M74" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B75" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75">
+        <v>650</v>
+      </c>
+      <c r="D75">
+        <v>75</v>
+      </c>
+      <c r="E75">
+        <v>50</v>
+      </c>
+      <c r="F75">
+        <v>6</v>
+      </c>
+      <c r="G75">
+        <v>60</v>
+      </c>
+      <c r="H75">
+        <v>2800</v>
+      </c>
+      <c r="I75">
+        <v>2800</v>
+      </c>
+      <c r="J75">
+        <v>133</v>
+      </c>
+      <c r="K75">
+        <v>2</v>
+      </c>
+      <c r="L75">
+        <v>0.6</v>
+      </c>
+      <c r="M75" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B76" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76">
+        <v>750</v>
+      </c>
+      <c r="D76">
+        <v>85</v>
+      </c>
+      <c r="E76">
+        <v>75</v>
+      </c>
+      <c r="F76">
+        <v>4</v>
+      </c>
+      <c r="G76">
+        <v>50</v>
+      </c>
+      <c r="H76">
+        <v>1750</v>
+      </c>
+      <c r="I76">
+        <v>1750</v>
+      </c>
+      <c r="J76">
+        <v>24</v>
+      </c>
+      <c r="K76">
+        <v>2</v>
+      </c>
+      <c r="L76">
+        <v>0.6</v>
+      </c>
+      <c r="M76" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B77" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77">
+        <v>850</v>
+      </c>
+      <c r="D77">
+        <v>95</v>
+      </c>
+      <c r="E77">
+        <v>85</v>
+      </c>
+      <c r="F77">
+        <v>8</v>
+      </c>
+      <c r="G77">
+        <v>60</v>
+      </c>
+      <c r="H77">
+        <v>4550</v>
+      </c>
+      <c r="I77">
+        <v>4550</v>
+      </c>
+      <c r="J77">
+        <v>24</v>
+      </c>
+      <c r="K77">
+        <v>2</v>
+      </c>
+      <c r="L77">
+        <v>0.6</v>
+      </c>
+      <c r="M77" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B78" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78">
+        <v>1200</v>
+      </c>
+      <c r="D78">
+        <v>100</v>
+      </c>
+      <c r="E78">
+        <v>50</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+      <c r="G78">
+        <v>90</v>
+      </c>
+      <c r="H78">
+        <v>4750</v>
+      </c>
+      <c r="I78">
+        <v>4750</v>
+      </c>
+      <c r="J78">
+        <v>56</v>
+      </c>
+      <c r="K78">
+        <v>5.5</v>
+      </c>
+      <c r="L78">
+        <v>0.65</v>
+      </c>
+      <c r="M78" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B79" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79">
+        <v>1400</v>
+      </c>
+      <c r="D79">
+        <v>110</v>
+      </c>
+      <c r="E79">
+        <v>65</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
+      </c>
+      <c r="G79">
+        <v>95</v>
+      </c>
+      <c r="H79">
+        <v>4950</v>
+      </c>
+      <c r="I79">
+        <v>4950</v>
+      </c>
+      <c r="J79">
+        <v>56</v>
+      </c>
+      <c r="K79">
+        <v>5.5</v>
+      </c>
+      <c r="L79">
+        <v>0.65</v>
+      </c>
+      <c r="M79" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B80" t="s">
+        <v>4</v>
+      </c>
+      <c r="C80">
+        <v>900</v>
+      </c>
+      <c r="D80">
+        <v>60</v>
+      </c>
+      <c r="E80">
+        <v>110</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+      <c r="G80">
+        <v>85</v>
+      </c>
+      <c r="H80">
+        <v>5450</v>
+      </c>
+      <c r="I80">
+        <v>5450</v>
+      </c>
+      <c r="J80">
+        <v>133</v>
+      </c>
+      <c r="K80">
+        <v>5.5</v>
+      </c>
+      <c r="L80">
+        <v>0.65</v>
+      </c>
+      <c r="M80" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B81" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81">
+        <v>900</v>
+      </c>
+      <c r="D81">
+        <v>60</v>
+      </c>
+      <c r="E81">
+        <v>110</v>
+      </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
+      <c r="G81">
+        <v>85</v>
+      </c>
+      <c r="H81">
+        <v>5450</v>
+      </c>
+      <c r="I81">
+        <v>5450</v>
+      </c>
+      <c r="J81">
+        <v>133</v>
+      </c>
+      <c r="K81">
+        <v>5.5</v>
+      </c>
+      <c r="L81">
+        <v>0.65</v>
+      </c>
+      <c r="M81" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B82" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82">
+        <v>1600</v>
+      </c>
+      <c r="D82">
+        <v>180</v>
+      </c>
+      <c r="E82">
+        <v>55</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>95</v>
+      </c>
+      <c r="H82">
+        <v>6550</v>
+      </c>
+      <c r="I82">
+        <v>6550</v>
+      </c>
+      <c r="J82">
+        <v>56</v>
+      </c>
+      <c r="K82">
+        <v>6</v>
+      </c>
+      <c r="L82">
+        <v>0.65</v>
+      </c>
+      <c r="M82" s="2">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:AO82" xr:uid="{0EFDF5D9-DFB6-4FE6-83FD-7EBB7A7830B6}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="(HA) BattleDragon"/>
+        <filter val="(HA) Beta"/>
+        <filter val="(HA) Charubah"/>
+        <filter val="(HA) Corona"/>
+        <filter val="(HA) Express"/>
+        <filter val="(HA) Flare"/>
+        <filter val="(HA) Magnetar"/>
+        <filter val="(HA) Mist"/>
+        <filter val="(HA) Neutron"/>
+        <filter val="(HA) NovaCruiser"/>
+        <filter val="(HA) Olanji"/>
+        <filter val="(HA) Pulsar"/>
+        <filter val="(HA) Ray"/>
+        <filter val="(HA) StarHome"/>
+        <filter val="(HA) Stella"/>
+        <filter val="(HA) Terephon"/>
+        <filter val="(IR) Allegiance"/>
+        <filter val="(IR) Altor"/>
+        <filter val="(IR) Carrack"/>
+        <filter val="(IR) Dreadnaught"/>
+        <filter val="(IR) EscortCarrier"/>
+        <filter val="(IR) Immobilizer"/>
+        <filter val="(IR) ISDI"/>
+        <filter val="(IR) ISDII"/>
+        <filter val="(IR) Katana"/>
+        <filter val="(IR) Lancer"/>
+        <filter val="(IR) MTC"/>
+        <filter val="(IR) Pellaeon"/>
+        <filter val="(IR) Strikecruiser"/>
+        <filter val="(IR) Thrawn"/>
+        <filter val="(IR) TorpedoSphere"/>
+        <filter val="(IR) VSDI"/>
+        <filter val="(IR) VSDII"/>
+        <filter val="(IR) WorldDevastator"/>
+        <filter val="(PA) Secutor"/>
+        <filter val="(PA) Venator"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:AO69">
     <sortCondition ref="F2:F69"/>
   </sortState>

</xml_diff>

<commit_message>
2nd update to Hapan Draft
</commit_message>
<xml_diff>
--- a/ShipStats.xlsx
+++ b/ShipStats.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="116">
   <si>
     <t>w1 Range</t>
   </si>
@@ -889,7 +889,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -898,6 +898,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1222,9 +1223,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AO82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="19" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K84" sqref="K84"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="19" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P94" sqref="P94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1872,7 +1873,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -3182,7 +3183,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>35</v>
       </c>
@@ -3286,7 +3287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>36</v>
       </c>
@@ -3348,7 +3349,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>37</v>
       </c>
@@ -3452,7 +3453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>38</v>
       </c>
@@ -3556,7 +3557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -3660,7 +3661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -3764,7 +3765,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>41</v>
       </c>
@@ -4324,7 +4325,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>95</v>
       </c>
@@ -4564,7 +4565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>70</v>
       </c>
@@ -5416,7 +5417,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>93</v>
       </c>
@@ -5505,7 +5506,7 @@
       <c r="AF45"/>
       <c r="AG45"/>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>94</v>
       </c>
@@ -5870,7 +5871,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>87</v>
       </c>
@@ -6244,7 +6245,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>97</v>
       </c>
@@ -6437,7 +6438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>50</v>
       </c>
@@ -6668,7 +6669,7 @@
         <v>8</v>
       </c>
       <c r="O58" s="1">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="P58" s="1">
         <v>0</v>
@@ -6707,7 +6708,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="59" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>92</v>
       </c>
@@ -6796,7 +6797,7 @@
       <c r="AF59"/>
       <c r="AG59"/>
     </row>
-    <row r="60" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>96</v>
       </c>
@@ -6974,7 +6975,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>98</v>
       </c>
@@ -7411,7 +7412,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>99</v>
       </c>
@@ -7681,7 +7682,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>42</v>
       </c>
@@ -7812,6 +7813,48 @@
       <c r="M71" s="2">
         <v>1</v>
       </c>
+      <c r="N71" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O71" s="1">
+        <v>35</v>
+      </c>
+      <c r="P71" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q71" s="1">
+        <v>0</v>
+      </c>
+      <c r="R71" s="1">
+        <v>0</v>
+      </c>
+      <c r="S71" s="1">
+        <v>10000</v>
+      </c>
+      <c r="T71" s="2">
+        <v>1</v>
+      </c>
+      <c r="U71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V71" s="8">
+        <v>0</v>
+      </c>
+      <c r="W71" s="1">
+        <v>0</v>
+      </c>
+      <c r="X71" s="8">
+        <v>8</v>
+      </c>
+      <c r="Y71" s="8">
+        <v>8</v>
+      </c>
+      <c r="Z71" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA71" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="72" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
@@ -7853,6 +7896,48 @@
       <c r="M72" s="2">
         <v>2</v>
       </c>
+      <c r="N72" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O72" s="1">
+        <v>35</v>
+      </c>
+      <c r="P72" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q72" s="1">
+        <v>0</v>
+      </c>
+      <c r="R72" s="1">
+        <v>0</v>
+      </c>
+      <c r="S72" s="1">
+        <v>10000</v>
+      </c>
+      <c r="T72" s="2">
+        <v>1</v>
+      </c>
+      <c r="U72" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V72" s="1">
+        <v>0</v>
+      </c>
+      <c r="W72" s="1">
+        <v>0</v>
+      </c>
+      <c r="X72" s="8">
+        <v>15</v>
+      </c>
+      <c r="Y72" s="8">
+        <v>15</v>
+      </c>
+      <c r="Z72" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA72" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="73" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
@@ -7894,6 +7979,27 @@
       <c r="M73" s="2">
         <v>1</v>
       </c>
+      <c r="N73" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O73" s="1">
+        <v>35</v>
+      </c>
+      <c r="P73" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q73" s="1">
+        <v>0</v>
+      </c>
+      <c r="R73" s="1">
+        <v>0</v>
+      </c>
+      <c r="S73" s="1">
+        <v>10000</v>
+      </c>
+      <c r="T73" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
@@ -7935,6 +8041,48 @@
       <c r="M74" s="2">
         <v>1</v>
       </c>
+      <c r="N74" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O74" s="1">
+        <v>180</v>
+      </c>
+      <c r="P74" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="1">
+        <v>0</v>
+      </c>
+      <c r="R74" s="1">
+        <v>0</v>
+      </c>
+      <c r="S74" s="1">
+        <v>10000</v>
+      </c>
+      <c r="T74" s="2">
+        <v>8</v>
+      </c>
+      <c r="U74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V74" s="8">
+        <v>0</v>
+      </c>
+      <c r="W74" s="1">
+        <v>0</v>
+      </c>
+      <c r="X74" s="8">
+        <v>8</v>
+      </c>
+      <c r="Y74" s="8">
+        <v>8</v>
+      </c>
+      <c r="Z74" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA74" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="75" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
@@ -7976,6 +8124,69 @@
       <c r="M75" s="2">
         <v>3</v>
       </c>
+      <c r="N75" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O75" s="1">
+        <v>220</v>
+      </c>
+      <c r="P75" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q75" s="1">
+        <v>0</v>
+      </c>
+      <c r="R75" s="1">
+        <v>0</v>
+      </c>
+      <c r="S75" s="1">
+        <v>10000</v>
+      </c>
+      <c r="T75" s="2">
+        <v>8</v>
+      </c>
+      <c r="U75" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V75" s="1">
+        <v>100</v>
+      </c>
+      <c r="W75" s="1">
+        <v>0</v>
+      </c>
+      <c r="X75" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y75" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z75" s="2">
+        <v>6</v>
+      </c>
+      <c r="AA75" s="2">
+        <v>6</v>
+      </c>
+      <c r="AB75" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC75" s="1">
+        <v>45</v>
+      </c>
+      <c r="AD75" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE75" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF75" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG75" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH75" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="76" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
@@ -8017,6 +8228,48 @@
       <c r="M76" s="2">
         <v>2</v>
       </c>
+      <c r="N76" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O76" s="1">
+        <v>220</v>
+      </c>
+      <c r="P76" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q76" s="1">
+        <v>0</v>
+      </c>
+      <c r="R76" s="1">
+        <v>0</v>
+      </c>
+      <c r="S76" s="1">
+        <v>10000</v>
+      </c>
+      <c r="T76" s="2">
+        <v>8</v>
+      </c>
+      <c r="U76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V76" s="1">
+        <v>100</v>
+      </c>
+      <c r="W76" s="1">
+        <v>0</v>
+      </c>
+      <c r="X76" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y76" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z76" s="2">
+        <v>6</v>
+      </c>
+      <c r="AA76" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="77" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
@@ -8058,6 +8311,69 @@
       <c r="M77" s="2">
         <v>3</v>
       </c>
+      <c r="N77" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O77" s="1">
+        <v>220</v>
+      </c>
+      <c r="P77" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q77" s="1">
+        <v>0</v>
+      </c>
+      <c r="R77" s="1">
+        <v>0</v>
+      </c>
+      <c r="S77" s="1">
+        <v>10000</v>
+      </c>
+      <c r="T77" s="2">
+        <v>8</v>
+      </c>
+      <c r="U77" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V77" s="1">
+        <v>100</v>
+      </c>
+      <c r="W77" s="1">
+        <v>0</v>
+      </c>
+      <c r="X77" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y77" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z77" s="2">
+        <v>8</v>
+      </c>
+      <c r="AA77" s="2">
+        <v>6</v>
+      </c>
+      <c r="AB77" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC77" s="1">
+        <v>220</v>
+      </c>
+      <c r="AD77" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE77" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF77" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG77" s="2">
+        <v>15</v>
+      </c>
+      <c r="AH77" s="2">
+        <v>30</v>
+      </c>
     </row>
     <row r="78" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
@@ -8099,6 +8415,69 @@
       <c r="M78" s="2">
         <v>3</v>
       </c>
+      <c r="N78" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O78" s="1">
+        <v>220</v>
+      </c>
+      <c r="P78" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q78" s="1">
+        <v>0</v>
+      </c>
+      <c r="R78" s="1">
+        <v>0</v>
+      </c>
+      <c r="S78" s="1">
+        <v>10000</v>
+      </c>
+      <c r="T78" s="2">
+        <v>8</v>
+      </c>
+      <c r="U78" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="V78" s="1">
+        <v>450</v>
+      </c>
+      <c r="W78" s="1">
+        <v>0</v>
+      </c>
+      <c r="X78" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y78" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z78" s="1">
+        <v>10000</v>
+      </c>
+      <c r="AA78" s="2">
+        <v>6</v>
+      </c>
+      <c r="AB78" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC78" s="1">
+        <v>220</v>
+      </c>
+      <c r="AD78" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE78" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF78" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG78" s="2">
+        <v>15</v>
+      </c>
+      <c r="AH78" s="2">
+        <v>12</v>
+      </c>
     </row>
     <row r="79" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
@@ -8140,6 +8519,69 @@
       <c r="M79" s="2">
         <v>3</v>
       </c>
+      <c r="N79" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O79" s="1">
+        <v>220</v>
+      </c>
+      <c r="P79" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q79" s="1">
+        <v>0</v>
+      </c>
+      <c r="R79" s="1">
+        <v>0</v>
+      </c>
+      <c r="S79" s="1">
+        <v>10000</v>
+      </c>
+      <c r="T79" s="2">
+        <v>8</v>
+      </c>
+      <c r="U79" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="V79" s="1">
+        <v>450</v>
+      </c>
+      <c r="W79" s="1">
+        <v>0</v>
+      </c>
+      <c r="X79" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y79" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z79" s="1">
+        <v>10000</v>
+      </c>
+      <c r="AA79" s="2">
+        <v>6</v>
+      </c>
+      <c r="AB79" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC79" s="1">
+        <v>220</v>
+      </c>
+      <c r="AD79" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE79" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF79" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG79" s="2">
+        <v>15</v>
+      </c>
+      <c r="AH79" s="2">
+        <v>12</v>
+      </c>
     </row>
     <row r="80" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
@@ -8181,8 +8623,50 @@
       <c r="M80" s="2">
         <v>3</v>
       </c>
+      <c r="N80" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O80" s="1">
+        <v>220</v>
+      </c>
+      <c r="P80" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q80" s="1">
+        <v>0</v>
+      </c>
+      <c r="R80" s="1">
+        <v>0</v>
+      </c>
+      <c r="S80" s="1">
+        <v>10000</v>
+      </c>
+      <c r="T80" s="2">
+        <v>8</v>
+      </c>
+      <c r="U80" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="V80" s="1">
+        <v>450</v>
+      </c>
+      <c r="W80" s="1">
+        <v>0</v>
+      </c>
+      <c r="X80" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y80" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z80" s="1">
+        <v>10000</v>
+      </c>
+      <c r="AA80" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>110</v>
       </c>
@@ -8222,8 +8706,50 @@
       <c r="M81" s="2">
         <v>3</v>
       </c>
+      <c r="N81" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O81" s="1">
+        <v>220</v>
+      </c>
+      <c r="P81" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q81" s="1">
+        <v>0</v>
+      </c>
+      <c r="R81" s="1">
+        <v>0</v>
+      </c>
+      <c r="S81" s="1">
+        <v>10000</v>
+      </c>
+      <c r="T81" s="2">
+        <v>8</v>
+      </c>
+      <c r="U81" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="V81" s="1">
+        <v>450</v>
+      </c>
+      <c r="W81" s="1">
+        <v>0</v>
+      </c>
+      <c r="X81" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y81" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z81" s="1">
+        <v>10000</v>
+      </c>
+      <c r="AA81" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>111</v>
       </c>
@@ -8262,6 +8788,69 @@
       </c>
       <c r="M82" s="2">
         <v>3</v>
+      </c>
+      <c r="N82" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O82" s="1">
+        <v>220</v>
+      </c>
+      <c r="P82" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q82" s="1">
+        <v>0</v>
+      </c>
+      <c r="R82" s="1">
+        <v>0</v>
+      </c>
+      <c r="S82" s="1">
+        <v>10000</v>
+      </c>
+      <c r="T82" s="2">
+        <v>8</v>
+      </c>
+      <c r="U82" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="V82" s="1">
+        <v>450</v>
+      </c>
+      <c r="W82" s="1">
+        <v>0</v>
+      </c>
+      <c r="X82" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y82" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z82" s="1">
+        <v>10000</v>
+      </c>
+      <c r="AA82" s="2">
+        <v>6</v>
+      </c>
+      <c r="AB82" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC82" s="1">
+        <v>220</v>
+      </c>
+      <c r="AD82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG82" s="2">
+        <v>15</v>
+      </c>
+      <c r="AH82" s="2">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -8284,26 +8873,6 @@
         <filter val="(HA) StarHome"/>
         <filter val="(HA) Stella"/>
         <filter val="(HA) Terephon"/>
-        <filter val="(IR) Allegiance"/>
-        <filter val="(IR) Altor"/>
-        <filter val="(IR) Carrack"/>
-        <filter val="(IR) Dreadnaught"/>
-        <filter val="(IR) EscortCarrier"/>
-        <filter val="(IR) Immobilizer"/>
-        <filter val="(IR) ISDI"/>
-        <filter val="(IR) ISDII"/>
-        <filter val="(IR) Katana"/>
-        <filter val="(IR) Lancer"/>
-        <filter val="(IR) MTC"/>
-        <filter val="(IR) Pellaeon"/>
-        <filter val="(IR) Strikecruiser"/>
-        <filter val="(IR) Thrawn"/>
-        <filter val="(IR) TorpedoSphere"/>
-        <filter val="(IR) VSDI"/>
-        <filter val="(IR) VSDII"/>
-        <filter val="(IR) WorldDevastator"/>
-        <filter val="(PA) Secutor"/>
-        <filter val="(PA) Venator"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Rebuffed Supply chain to 5.0 from 1.0 previously nerfed from 50.0
</commit_message>
<xml_diff>
--- a/ShipStats.xlsx
+++ b/ShipStats.xlsx
@@ -712,7 +712,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1231,8 +1231,8 @@
   <dimension ref="A1:AO82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="19" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A77" sqref="A77"/>
+      <pane ySplit="19" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W94" sqref="W94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,7 +1402,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>44</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>49</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>114</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>46</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>47</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>45</v>
       </c>
@@ -5216,8 +5216,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+    <row r="43" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
         <v>115</v>
       </c>
       <c r="B43" t="s">
@@ -5691,7 +5691,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="48" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>51</v>
       </c>
@@ -5961,8 +5961,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+    <row r="51" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
         <v>113</v>
       </c>
       <c r="B51" t="s">
@@ -6341,7 +6341,7 @@
       <c r="AF54"/>
       <c r="AG54"/>
     </row>
-    <row r="55" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>48</v>
       </c>
@@ -6445,7 +6445,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>50</v>
       </c>
@@ -6510,7 +6510,7 @@
         <v>7</v>
       </c>
       <c r="V56" s="1">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="W56" s="1">
         <v>0</v>
@@ -7772,7 +7772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>100</v>
       </c>
@@ -7780,8 +7780,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+    <row r="71" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
         <v>101</v>
       </c>
       <c r="B71" t="s">
@@ -7863,8 +7863,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+    <row r="72" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
         <v>102</v>
       </c>
       <c r="B72" t="s">
@@ -7946,8 +7946,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+    <row r="73" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
         <v>103</v>
       </c>
       <c r="B73" t="s">
@@ -8008,8 +8008,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+    <row r="74" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="9" t="s">
         <v>104</v>
       </c>
       <c r="B74" t="s">
@@ -8091,8 +8091,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+    <row r="75" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
         <v>105</v>
       </c>
       <c r="B75" t="s">
@@ -8195,8 +8195,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+    <row r="76" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
         <v>106</v>
       </c>
       <c r="B76" t="s">
@@ -8278,7 +8278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>107</v>
       </c>
@@ -8382,7 +8382,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>112</v>
       </c>
@@ -8486,7 +8486,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>108</v>
       </c>
@@ -8590,7 +8590,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>109</v>
       </c>
@@ -8673,7 +8673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>110</v>
       </c>
@@ -8756,7 +8756,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>111</v>
       </c>
@@ -8864,22 +8864,20 @@
   <autoFilter ref="A1:AO82" xr:uid="{0EFDF5D9-DFB6-4FE6-83FD-7EBB7A7830B6}">
     <filterColumn colId="0">
       <filters>
-        <filter val="(HA) BattleDragon"/>
-        <filter val="(HA) Beta"/>
-        <filter val="(HA) Charubah"/>
-        <filter val="(HA) Corona"/>
-        <filter val="(HA) Express"/>
-        <filter val="(HA) Flare"/>
-        <filter val="(HA) Magnetar"/>
-        <filter val="(HA) Mist"/>
-        <filter val="(HA) Neutron"/>
-        <filter val="(HA) NovaCruiser"/>
-        <filter val="(HA) Olanji"/>
-        <filter val="(HA) Pulsar"/>
-        <filter val="(HA) Ray"/>
-        <filter val="(HA) StarHome"/>
-        <filter val="(HA) Stella"/>
-        <filter val="(HA) Terephon"/>
+        <filter val="(PA) Arquitens"/>
+        <filter val="(PA) Dominator"/>
+        <filter val="(PA) Enforcer"/>
+        <filter val="(PA) Gladiator"/>
+        <filter val="(PA) ISDI"/>
+        <filter val="(PA) ISDII"/>
+        <filter val="(PA) Lucrehulk"/>
+        <filter val="(PA) Munificent"/>
+        <filter val="(PA) Praetor"/>
+        <filter val="(PA) Procursator"/>
+        <filter val="(PA) Raider"/>
+        <filter val="(PA) Secutor"/>
+        <filter val="(PA) Venator"/>
+        <filter val="(PA) Vindicator"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>